<commit_message>
added doubly reinforced rcc beam design
</commit_message>
<xml_diff>
--- a/Structural design sheets/Beam design.xlsx
+++ b/Structural design sheets/Beam design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Structural design sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Exceldesignfiles\Structural design sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07D6F71-C171-4C74-A4B1-56D1B3A93768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5DFE61-30CE-4B29-AD3D-B267FF597592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{080EB4DA-FCC7-4271-9359-BF29FD8446FC}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <author>Samyak</author>
   </authors>
   <commentList>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{A94A0C6E-5B0B-4D0F-B511-9E983DEA732B}">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{A94A0C6E-5B0B-4D0F-B511-9E983DEA732B}">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>I - section</t>
   </si>
@@ -245,18 +245,6 @@
     <t>No of Rebar</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Rectangular beam, singly reinforced</t>
   </si>
   <si>
@@ -276,14 +264,55 @@
   </si>
   <si>
     <t>section moment calculation</t>
+  </si>
+  <si>
+    <t>Rectangular beam, doubly reinforced</t>
+  </si>
+  <si>
+    <t>d'</t>
+  </si>
+  <si>
+    <t>cover (t)</t>
+  </si>
+  <si>
+    <t>Compression reinforcement</t>
+  </si>
+  <si>
+    <t>Tension reinforcement</t>
+  </si>
+  <si>
+    <t>Asc provided</t>
+  </si>
+  <si>
+    <t>Esc</t>
+  </si>
+  <si>
+    <t>fsc</t>
+  </si>
+  <si>
+    <t>fcc</t>
+  </si>
+  <si>
+    <t>fst</t>
+  </si>
+  <si>
+    <t>xu lim</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>kNm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -329,7 +358,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -353,9 +382,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -366,7 +393,44 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -374,7 +438,71 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -387,9 +515,46 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -398,42 +563,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -453,28 +614,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -577,11 +800,201 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -938,7 +1351,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF0584A-E401-4C04-B945-1304245BCBFF}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1593,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1209,7 +1622,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>415</v>
@@ -1235,19 +1648,24 @@
         <v>19.82</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>42</v>
       </c>
       <c r="R4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="19"/>
+      <c r="A5" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1256,29 +1674,17 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="18" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="27"/>
+      <c r="I6" s="15" t="s">
         <v>55</v>
       </c>
       <c r="J6" s="6">
@@ -1297,339 +1703,927 @@
         <v>32</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>300</v>
-      </c>
-      <c r="B7" s="13">
-        <f>SQRT(E7*1000000/(F3*A3*A7))</f>
-        <v>491.47318718299044</v>
-      </c>
-      <c r="C7" s="6">
-        <v>650</v>
-      </c>
-      <c r="D7">
-        <f>C7+50</f>
-        <v>700</v>
-      </c>
-      <c r="E7">
+      <c r="A7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="15">
+        <v>2</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" ref="J7:N11" si="0">PI()*J$6^2/4*$I7</f>
+        <v>226.1946710584651</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="0"/>
+        <v>402.12385965949352</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="0"/>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="0"/>
+        <v>981.74770424681037</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="0"/>
+        <v>1608.4954386379741</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>230</v>
+      </c>
+      <c r="B8" s="11">
+        <f>SQRT(E8*1000000/(F3*A3*A8))</f>
+        <v>627.55464042350627</v>
+      </c>
+      <c r="C8" s="6">
+        <v>675</v>
+      </c>
+      <c r="D8" s="12">
+        <f>C8+50</f>
+        <v>725</v>
+      </c>
+      <c r="E8" s="12">
         <v>250</v>
       </c>
-      <c r="F7">
-        <f>F3*A3*A7*C7^2/1000000</f>
-        <v>437.28750000000002</v>
-      </c>
-      <c r="I7" s="18">
-        <v>2</v>
-      </c>
-      <c r="J7" s="17">
-        <f>PI()*J$6^2/4*$I7</f>
-        <v>226.1946710584651</v>
-      </c>
-      <c r="K7" s="17">
-        <f>PI()*K$6^2/4*$I7</f>
-        <v>402.12385965949352</v>
-      </c>
-      <c r="L7" s="17">
-        <f>PI()*L$6^2/4*$I7</f>
-        <v>628.31853071795865</v>
-      </c>
-      <c r="M7" s="17">
-        <f>PI()*M$6^2/4*$I7</f>
-        <v>981.74770424681037</v>
-      </c>
-      <c r="N7" s="17">
-        <f>PI()*N$6^2/4*$I7</f>
-        <v>1608.4954386379741</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>29</v>
+      <c r="F8" s="27">
+        <f>F3*A3*A8*C8^2/1000000</f>
+        <v>289.23075000000006</v>
       </c>
       <c r="I8" s="6">
         <v>3</v>
       </c>
-      <c r="J8" s="17">
-        <f>PI()*J$6^2/4*$I8</f>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
         <v>339.29200658769764</v>
       </c>
-      <c r="K8" s="17">
-        <f>PI()*K$6^2/4*$I8</f>
+      <c r="K8" s="14">
+        <f t="shared" si="0"/>
         <v>603.18578948924028</v>
       </c>
-      <c r="L8" s="17">
-        <f>PI()*L$6^2/4*$I8</f>
+      <c r="L8" s="14">
+        <f t="shared" si="0"/>
         <v>942.47779607693792</v>
       </c>
-      <c r="M8" s="17">
-        <f>PI()*M$6^2/4*$I8</f>
+      <c r="M8" s="14">
+        <f t="shared" si="0"/>
         <v>1472.6215563702156</v>
       </c>
-      <c r="N8" s="17">
-        <f>PI()*N$6^2/4*$I8</f>
+      <c r="N8" s="14">
+        <f t="shared" si="0"/>
         <v>2412.7431579569611</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="27"/>
       <c r="I9" s="6">
         <v>4</v>
       </c>
-      <c r="J9" s="17">
-        <f>PI()*J$6^2/4*$I9</f>
+      <c r="J9" s="14">
+        <f t="shared" si="0"/>
         <v>452.38934211693021</v>
       </c>
-      <c r="K9" s="17">
-        <f>PI()*K$6^2/4*$I9</f>
+      <c r="K9" s="14">
+        <f t="shared" si="0"/>
         <v>804.24771931898704</v>
       </c>
-      <c r="L9" s="17">
-        <f>PI()*L$6^2/4*$I9</f>
+      <c r="L9" s="14">
+        <f t="shared" si="0"/>
         <v>1256.6370614359173</v>
       </c>
-      <c r="M9" s="17">
-        <f>PI()*M$6^2/4*$I9</f>
+      <c r="M9" s="14">
+        <f t="shared" si="0"/>
         <v>1963.4954084936207</v>
       </c>
-      <c r="N9" s="17">
-        <f>PI()*N$6^2/4*$I9</f>
+      <c r="N9" s="14">
+        <f t="shared" si="0"/>
         <v>3216.9908772759482</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <f>G3*A3/B3</f>
-        <v>1.1939759036144579</v>
-      </c>
-      <c r="B10" s="7">
-        <f>A10/100*A7*C7</f>
-        <v>2328.2530120481929</v>
-      </c>
-      <c r="C10" s="17">
-        <v>1256.6400000000001</v>
-      </c>
-      <c r="D10" s="7">
-        <f>MAX(0.25*SQRT(A3)/B3,1.4/B3)*A7*C7</f>
-        <v>657.83132530120474</v>
-      </c>
-      <c r="E10" t="str">
-        <f>IF(C10&lt;B10, "under-reinforced","over-reinforced")</f>
-        <v>under-reinforced</v>
-      </c>
+      <c r="A10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="27"/>
       <c r="I10" s="6">
         <v>5</v>
       </c>
-      <c r="J10" s="17">
-        <f>PI()*J$6^2/4*$I10</f>
+      <c r="J10" s="14">
+        <f t="shared" si="0"/>
         <v>565.48667764616278</v>
       </c>
-      <c r="K10" s="17">
-        <f>PI()*K$6^2/4*$I10</f>
+      <c r="K10" s="14">
+        <f t="shared" si="0"/>
         <v>1005.3096491487338</v>
       </c>
-      <c r="L10" s="17">
-        <f>PI()*L$6^2/4*$I10</f>
+      <c r="L10" s="14">
+        <f t="shared" si="0"/>
         <v>1570.7963267948967</v>
       </c>
-      <c r="M10" s="17">
-        <f>PI()*M$6^2/4*$I10</f>
+      <c r="M10" s="14">
+        <f t="shared" si="0"/>
         <v>2454.3692606170262</v>
       </c>
-      <c r="N10" s="17">
-        <f>PI()*N$6^2/4*$I10</f>
+      <c r="N10" s="14">
+        <f t="shared" si="0"/>
         <v>4021.2385965949352</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="30">
+        <f>G3*A3/B3</f>
+        <v>0.95518072289156619</v>
+      </c>
+      <c r="B11" s="11">
+        <f>A11/100*A8*C8</f>
+        <v>1482.9180722891565</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1256.6400000000001</v>
+      </c>
+      <c r="D11" s="11">
+        <f>MAX(0.25*SQRT(A3)/B3,1.4/B3)*A8*C8</f>
+        <v>523.73493975903614</v>
+      </c>
+      <c r="E11" s="12" t="str">
+        <f>IF(C11&lt;B11, "under-reinforced","over-reinforced")</f>
+        <v>under-reinforced</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="I11" s="15">
+        <v>6</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="0"/>
+        <v>678.58401317539528</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="0"/>
+        <v>1206.3715789784806</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="0"/>
+        <v>1884.9555921538758</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="0"/>
+        <v>2945.2431127404311</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="0"/>
+        <v>4825.4863159139222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <f>0.87*B3*C11</f>
+        <v>453709.87200000003</v>
+      </c>
+      <c r="B15" s="13">
+        <f>0.36*A3*A8</f>
+        <v>1655.9999999999998</v>
+      </c>
+      <c r="C15" s="17">
+        <f>A15/B15</f>
+        <v>273.97939130434787</v>
+      </c>
+      <c r="D15" s="17">
+        <f>C8*(1-0.416*C15/C8)</f>
+        <v>561.02457321739132</v>
+      </c>
+      <c r="E15" s="20">
+        <f>A15*D15/1000000</f>
+        <v>254.54238730331724</v>
+      </c>
+      <c r="F15" s="36">
+        <f>C15/C8</f>
+        <v>0.40589539452495982</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="27"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="33"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="35">
+        <f>0.87*B3*C11</f>
+        <v>453709.87200000003</v>
+      </c>
+      <c r="B19" s="13">
+        <f>0.45*A3*A8</f>
+        <v>2070</v>
+      </c>
+      <c r="C19" s="17">
+        <f>A19/B19</f>
+        <v>219.18351304347829</v>
+      </c>
+      <c r="D19" s="17">
+        <f>C8-C19/2</f>
+        <v>565.40824347826083</v>
+      </c>
+      <c r="E19" s="21">
+        <f>A19*D19/1000000</f>
+        <v>256.53130177626656</v>
+      </c>
+      <c r="F19" s="36">
+        <f>C19/C8</f>
+        <v>0.32471631561996783</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="27"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
+        <v>230</v>
+      </c>
+      <c r="B25" s="6">
+        <v>500</v>
+      </c>
+      <c r="C25" s="12">
+        <v>30</v>
+      </c>
+      <c r="D25" s="12">
+        <v>50</v>
+      </c>
+      <c r="E25" s="12">
+        <f>B25+D25</f>
+        <v>550</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="27"/>
+      <c r="K25" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" s="6">
+        <v>12</v>
+      </c>
+      <c r="M25" s="6">
+        <v>16</v>
+      </c>
+      <c r="N25" s="6">
+        <v>20</v>
+      </c>
+      <c r="O25" s="6">
+        <v>25</v>
+      </c>
+      <c r="P25" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="27"/>
+      <c r="K26" s="15">
+        <v>2</v>
+      </c>
+      <c r="L26" s="14">
+        <f>PI()*L$25^2/4*$K26</f>
+        <v>226.1946710584651</v>
+      </c>
+      <c r="M26" s="14">
+        <f t="shared" ref="M26:P30" si="1">PI()*M$25^2/4*$K26</f>
+        <v>402.12385965949352</v>
+      </c>
+      <c r="N26" s="14">
+        <f t="shared" si="1"/>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="O26" s="14">
+        <f t="shared" si="1"/>
+        <v>981.74770424681037</v>
+      </c>
+      <c r="P26" s="14">
+        <f t="shared" si="1"/>
+        <v>1608.4954386379741</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="14"/>
-      <c r="I11" s="18">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="6">
+        <v>3</v>
+      </c>
+      <c r="L27" s="14">
+        <f t="shared" ref="L27:L30" si="2">PI()*L$25^2/4*$K27</f>
+        <v>339.29200658769764</v>
+      </c>
+      <c r="M27" s="14">
+        <f t="shared" si="1"/>
+        <v>603.18578948924028</v>
+      </c>
+      <c r="N27" s="14">
+        <f t="shared" si="1"/>
+        <v>942.47779607693792</v>
+      </c>
+      <c r="O27" s="14">
+        <f t="shared" si="1"/>
+        <v>1472.6215563702156</v>
+      </c>
+      <c r="P27" s="14">
+        <f t="shared" si="1"/>
+        <v>2412.7431579569611</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12">
+        <f>C29</f>
+        <v>239.5</v>
+      </c>
+      <c r="G28" s="42">
+        <f>0.0035*(F28-$C$25)/F28</f>
+        <v>3.0615866388308982E-3</v>
+      </c>
+      <c r="H28" s="43">
+        <f>IF($B$3=415,-109.1569+537276.6*G28-250905000*G28^2+55282490000*G28^3-4709357000000*G28^4,1707.624-2356626*G28-1444077000*G28^2+366690400000*G28^3-33180890000000*G28^4)</f>
+        <v>356.6447401411944</v>
+      </c>
+      <c r="I28" s="44">
+        <f>($A$32*$B$32-(H28-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>173.60825454972272</v>
+      </c>
+      <c r="K28" s="6">
+        <v>4</v>
+      </c>
+      <c r="L28" s="14">
+        <f t="shared" si="2"/>
+        <v>452.38934211693021</v>
+      </c>
+      <c r="M28" s="14">
+        <f t="shared" si="1"/>
+        <v>804.24771931898704</v>
+      </c>
+      <c r="N28" s="14">
+        <f t="shared" si="1"/>
+        <v>1256.6370614359173</v>
+      </c>
+      <c r="O28" s="14">
+        <f t="shared" si="1"/>
+        <v>1963.4954084936207</v>
+      </c>
+      <c r="P28" s="14">
+        <f t="shared" si="1"/>
+        <v>3216.9908772759482</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <f>M28</f>
+        <v>804.24771931898704</v>
+      </c>
+      <c r="B29" s="12">
+        <f>0.447*A3</f>
+        <v>8.94</v>
+      </c>
+      <c r="C29" s="12">
+        <f>C3*B25</f>
+        <v>239.5</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="11">
+        <f>I28</f>
+        <v>173.60825454972272</v>
+      </c>
+      <c r="G29" s="42">
+        <f>0.0035*(F29-$C$25)/F29</f>
+        <v>2.8951900485818939E-3</v>
+      </c>
+      <c r="H29" s="43">
+        <f>IF($B$3=415,-109.1569+537276.6*G29-250905000*G29^2+55282490000*G29^3-4709357000000*G29^4,1707.624-2356626*G29-1444077000*G29^2+366690400000*G29^3-33180890000000*G29^4)</f>
+        <v>353.95119915899562</v>
+      </c>
+      <c r="I29" s="44">
+        <f>($A$32*$B$32-(H29-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.91639113898938</v>
+      </c>
+      <c r="K29" s="6">
+        <v>5</v>
+      </c>
+      <c r="L29" s="14">
+        <f t="shared" si="2"/>
+        <v>565.48667764616278</v>
+      </c>
+      <c r="M29" s="14">
+        <f t="shared" si="1"/>
+        <v>1005.3096491487338</v>
+      </c>
+      <c r="N29" s="14">
+        <f t="shared" si="1"/>
+        <v>1570.7963267948967</v>
+      </c>
+      <c r="O29" s="14">
+        <f t="shared" si="1"/>
+        <v>2454.3692606170262</v>
+      </c>
+      <c r="P29" s="14">
+        <f t="shared" si="1"/>
+        <v>4021.2385965949352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="11">
+        <f t="shared" ref="F30:F32" si="3">I29</f>
+        <v>174.91639113898938</v>
+      </c>
+      <c r="G30" s="42">
+        <f t="shared" ref="G30:G32" si="4">0.0035*(F30-$C$25)/F30</f>
+        <v>2.8997132040269086E-3</v>
+      </c>
+      <c r="H30" s="43">
+        <f t="shared" ref="H30:H32" si="5">IF($B$3=415,-109.1569+537276.6*G30-250905000*G30^2+55282490000*G30^3-4709357000000*G30^4,1707.624-2356626*G30-1444077000*G30^2+366690400000*G30^3-33180890000000*G30^4)</f>
+        <v>354.02998098735662</v>
+      </c>
+      <c r="I30" s="44">
+        <f t="shared" ref="I30:I32" si="6">($A$32*$B$32-(H30-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87813020554546</v>
+      </c>
+      <c r="K30" s="15">
         <v>6</v>
       </c>
-      <c r="J11" s="17">
-        <f>PI()*J$6^2/4*$I11</f>
+      <c r="L30" s="14">
+        <f t="shared" si="2"/>
         <v>678.58401317539528</v>
       </c>
-      <c r="K11" s="17">
-        <f>PI()*K$6^2/4*$I11</f>
+      <c r="M30" s="14">
+        <f t="shared" si="1"/>
         <v>1206.3715789784806</v>
       </c>
-      <c r="L11" s="17">
-        <f>PI()*L$6^2/4*$I11</f>
+      <c r="N30" s="14">
+        <f t="shared" si="1"/>
         <v>1884.9555921538758</v>
       </c>
-      <c r="M11" s="17">
-        <f>PI()*M$6^2/4*$I11</f>
+      <c r="O30" s="14">
+        <f t="shared" si="1"/>
         <v>2945.2431127404311</v>
       </c>
-      <c r="N11" s="17">
-        <f>PI()*N$6^2/4*$I11</f>
+      <c r="P30" s="14">
+        <f t="shared" si="1"/>
         <v>4825.4863159139222</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <f>0.87*B3*C10</f>
-        <v>453709.87200000003</v>
-      </c>
-      <c r="B14" s="16">
-        <f>0.36*A3*A7</f>
-        <v>2700</v>
-      </c>
-      <c r="C14" s="20">
-        <f>A14/B14</f>
-        <v>168.04069333333334</v>
-      </c>
-      <c r="D14" s="20">
-        <f>C7*(1-0.416*C14/C7)</f>
-        <v>580.09507157333337</v>
-      </c>
-      <c r="E14" s="24">
-        <f>A14*D14/1000000</f>
-        <v>263.19486067136796</v>
-      </c>
-      <c r="F14" s="22">
-        <f>C14/C7</f>
-        <v>0.25852414358974357</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <f>0.87*B3*C10</f>
-        <v>453709.87200000003</v>
-      </c>
-      <c r="B18" s="16">
-        <f>0.45*A3*A7</f>
-        <v>3375</v>
-      </c>
-      <c r="C18" s="20">
-        <f>A18/B18</f>
-        <v>134.43255466666668</v>
-      </c>
-      <c r="D18" s="20">
-        <f>C7-C18/2</f>
-        <v>582.78372266666668</v>
-      </c>
-      <c r="E18" s="25">
-        <f>A18*D18/1000000</f>
-        <v>264.41472821477686</v>
-      </c>
-      <c r="F18" s="22">
-        <f>C18/C7</f>
-        <v>0.20681931487179489</v>
-      </c>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="11">
+        <f t="shared" si="3"/>
+        <v>174.87813020554546</v>
+      </c>
+      <c r="G31" s="42">
+        <f t="shared" si="4"/>
+        <v>2.8995818695191516E-3</v>
+      </c>
+      <c r="H31" s="43">
+        <f t="shared" si="5"/>
+        <v>354.02769785043228</v>
+      </c>
+      <c r="I31" s="44">
+        <f t="shared" si="6"/>
+        <v>174.87923902659878</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <f>N29</f>
+        <v>1570.7963267948967</v>
+      </c>
+      <c r="B32" s="12">
+        <f>0.87*B3</f>
+        <v>361.05</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="11">
+        <f t="shared" si="3"/>
+        <v>174.87923902659878</v>
+      </c>
+      <c r="G32" s="42">
+        <f t="shared" si="4"/>
+        <v>2.8995856764676927E-3</v>
+      </c>
+      <c r="H32" s="43">
+        <f t="shared" si="5"/>
+        <v>354.02776403462366</v>
+      </c>
+      <c r="I32" s="44">
+        <f t="shared" si="6"/>
+        <v>174.87920688379387</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="11">
+        <f>I32</f>
+        <v>174.87920688379387</v>
+      </c>
+      <c r="G33" s="42">
+        <f>0.0035*(F33-$C$25)/F33</f>
+        <v>2.8995855661115171E-3</v>
+      </c>
+      <c r="H33" s="43">
+        <f>IF($B$3=415,-109.1569+537276.6*G33-250905000*G33^2+55282490000*G33^3-4709357000000*G33^4,1707.624-2356626*G33-1444077000*G33^2+366690400000*G33^3-33180890000000*G33^4)</f>
+        <v>354.02776211607318</v>
+      </c>
+      <c r="I33" s="44">
+        <f>($A$32*$B$32-(H33-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87920781555101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="11">
+        <f>I33</f>
+        <v>174.87920781555101</v>
+      </c>
+      <c r="G34" s="42">
+        <f>0.0035*(F34-$C$25)/F34</f>
+        <v>2.8995855693105272E-3</v>
+      </c>
+      <c r="H34" s="43">
+        <f>IF($B$3=415,-109.1569+537276.6*G34-250905000*G34^2+55282490000*G34^3-4709357000000*G34^4,1707.624-2356626*G34-1444077000*G34^2+366690400000*G34^3-33180890000000*G34^4)</f>
+        <v>354.02776217168855</v>
+      </c>
+      <c r="I34" s="44">
+        <f>($A$32*$B$32-(H34-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87920778854104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="11">
+        <f>(0.36*A3*A25*I38*(B25-0.416*I38)+(H38-B29)*A29*(B25-C25))/1000000</f>
+        <v>254.17360011720072</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="11">
+        <f t="shared" ref="F35:F37" si="7">I34</f>
+        <v>174.87920778854104</v>
+      </c>
+      <c r="G35" s="42">
+        <f t="shared" ref="G35:G37" si="8">0.0035*(F35-$C$25)/F35</f>
+        <v>2.8995855692177941E-3</v>
+      </c>
+      <c r="H35" s="43">
+        <f t="shared" ref="H35:H37" si="9">IF($B$3=415,-109.1569+537276.6*G35-250905000*G35^2+55282490000*G35^3-4709357000000*G35^4,1707.624-2356626*G35-1444077000*G35^2+366690400000*G35^3-33180890000000*G35^4)</f>
+        <v>354.02776217007596</v>
+      </c>
+      <c r="I35" s="44">
+        <f t="shared" ref="I35:I37" si="10">($A$32*$B$32-(H35-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.8792077893242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="11">
+        <f t="shared" si="7"/>
+        <v>174.8792077893242</v>
+      </c>
+      <c r="G36" s="42">
+        <f t="shared" si="8"/>
+        <v>2.8995855692204829E-3</v>
+      </c>
+      <c r="H36" s="43">
+        <f t="shared" si="9"/>
+        <v>354.02776217012297</v>
+      </c>
+      <c r="I36" s="44">
+        <f t="shared" si="10"/>
+        <v>174.87920778930135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="11">
+        <f t="shared" si="7"/>
+        <v>174.87920778930135</v>
+      </c>
+      <c r="G37" s="42">
+        <f t="shared" si="8"/>
+        <v>2.8995855692204048E-3</v>
+      </c>
+      <c r="H37" s="43">
+        <f t="shared" si="9"/>
+        <v>354.02776217012172</v>
+      </c>
+      <c r="I37" s="44">
+        <f t="shared" si="10"/>
+        <v>174.87920778930197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="45">
+        <f>I37</f>
+        <v>174.87920778930197</v>
+      </c>
+      <c r="G38" s="46">
+        <f>0.0035*(F38-$C$25)/F38</f>
+        <v>2.8995855692204066E-3</v>
+      </c>
+      <c r="H38" s="47">
+        <f>IF($B$3=415,-109.1569+537276.6*G38-250905000*G38^2+55282490000*G38^3-4709357000000*G38^4,1707.624-2356626*G38-1444077000*G38^2+366690400000*G38^3-33180890000000*G38^4)</f>
+        <v>354.02776217012138</v>
+      </c>
+      <c r="I38" s="48">
+        <f>($A$32*$B$32-(H38-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87920778930211</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:N11">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
-      <formula>$D$10</formula>
-      <formula>$B$10</formula>
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="between">
+      <formula>$D$11</formula>
+      <formula>$B$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
       <formula>"over-reinforced"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
-      <formula>$C$10</formula>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
+      <formula>$C$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
-      <formula>$C$10</formula>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="lessThan">
+      <formula>$C$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>$B$7</formula>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="lessThan">
+      <formula>$B$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18 E14">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="lessThan">
-      <formula>$E$7</formula>
+  <conditionalFormatting sqref="E19 E15">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="lessThan">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46 I28:I38">
+    <cfRule type="cellIs" dxfId="17" priority="12" operator="greaterThan">
+      <formula>$C$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:I38">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$C$29</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
1. added provision to calculate reinforcement in a singly reinforced beam 2. Cantilever retaining wall design. Procedure followed from Subramanyam RCC book 3. Corresponding autocad drawing of cantilever retaining wall
</commit_message>
<xml_diff>
--- a/Structural design sheets/Beam design.xlsx
+++ b/Structural design sheets/Beam design.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Exceldesignfiles\Structural design sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5DFE61-30CE-4B29-AD3D-B267FF597592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F751061-6297-4136-8668-8DDDFA760EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{080EB4DA-FCC7-4271-9359-BF29FD8446FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Steel" sheetId="1" r:id="rId1"/>
     <sheet name="RCC" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="bf">Steel!$C$3</definedName>
@@ -74,8 +75,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>I - section</t>
   </si>
@@ -303,6 +326,51 @@
   </si>
   <si>
     <t>kNm</t>
+  </si>
+  <si>
+    <t>Ast</t>
+  </si>
+  <si>
+    <t>Ast'=Mu/0.87fy(d-0.416xu)</t>
+  </si>
+  <si>
+    <t>Ast for moment</t>
+  </si>
+  <si>
+    <t>Ast required=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provide </t>
+  </si>
+  <si>
+    <t>Ast provided =</t>
+  </si>
+  <si>
+    <t>Mu required</t>
+  </si>
+  <si>
+    <t>clear cover</t>
+  </si>
+  <si>
+    <t>use bar of dia</t>
+  </si>
+  <si>
+    <t>d min</t>
+  </si>
+  <si>
+    <t>Find Ast in singly reinforced beam for a given Mu and beam width</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>no of bars=</t>
+  </si>
+  <si>
+    <t>spacing=</t>
+  </si>
+  <si>
+    <t>mm c/c</t>
   </si>
 </sst>
 </file>
@@ -311,8 +379,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -358,7 +426,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -590,11 +658,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -643,21 +759,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -675,306 +799,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,10 +1400,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF0584A-E401-4C04-B945-1304245BCBFF}">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,6 +1413,7 @@
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
@@ -2195,7 +2021,7 @@
       <c r="H27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I27" s="49" t="s">
+      <c r="I27" s="47" t="s">
         <v>44</v>
       </c>
       <c r="K27" s="6">
@@ -2238,15 +2064,15 @@
         <f>C29</f>
         <v>239.5</v>
       </c>
-      <c r="G28" s="42">
+      <c r="G28" s="40">
         <f>0.0035*(F28-$C$25)/F28</f>
         <v>3.0615866388308982E-3</v>
       </c>
-      <c r="H28" s="43">
+      <c r="H28" s="41">
         <f>IF($B$3=415,-109.1569+537276.6*G28-250905000*G28^2+55282490000*G28^3-4709357000000*G28^4,1707.624-2356626*G28-1444077000*G28^2+366690400000*G28^3-33180890000000*G28^4)</f>
         <v>356.6447401411944</v>
       </c>
-      <c r="I28" s="44">
+      <c r="I28" s="42">
         <f>($A$32*$B$32-(H28-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
         <v>173.60825454972272</v>
       </c>
@@ -2293,15 +2119,15 @@
         <f>I28</f>
         <v>173.60825454972272</v>
       </c>
-      <c r="G29" s="42">
+      <c r="G29" s="40">
         <f>0.0035*(F29-$C$25)/F29</f>
         <v>2.8951900485818939E-3</v>
       </c>
-      <c r="H29" s="43">
+      <c r="H29" s="41">
         <f>IF($B$3=415,-109.1569+537276.6*G29-250905000*G29^2+55282490000*G29^3-4709357000000*G29^4,1707.624-2356626*G29-1444077000*G29^2+366690400000*G29^3-33180890000000*G29^4)</f>
         <v>353.95119915899562</v>
       </c>
-      <c r="I29" s="44">
+      <c r="I29" s="42">
         <f>($A$32*$B$32-(H29-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
         <v>174.91639113898938</v>
       </c>
@@ -2341,15 +2167,15 @@
         <f t="shared" ref="F30:F32" si="3">I29</f>
         <v>174.91639113898938</v>
       </c>
-      <c r="G30" s="42">
+      <c r="G30" s="40">
         <f t="shared" ref="G30:G32" si="4">0.0035*(F30-$C$25)/F30</f>
         <v>2.8997132040269086E-3</v>
       </c>
-      <c r="H30" s="43">
+      <c r="H30" s="41">
         <f t="shared" ref="H30:H32" si="5">IF($B$3=415,-109.1569+537276.6*G30-250905000*G30^2+55282490000*G30^3-4709357000000*G30^4,1707.624-2356626*G30-1444077000*G30^2+366690400000*G30^3-33180890000000*G30^4)</f>
         <v>354.02998098735662</v>
       </c>
-      <c r="I30" s="44">
+      <c r="I30" s="42">
         <f t="shared" ref="I30:I32" si="6">($A$32*$B$32-(H30-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
         <v>174.87813020554546</v>
       </c>
@@ -2391,15 +2217,15 @@
         <f t="shared" si="3"/>
         <v>174.87813020554546</v>
       </c>
-      <c r="G31" s="42">
+      <c r="G31" s="40">
         <f t="shared" si="4"/>
         <v>2.8995818695191516E-3</v>
       </c>
-      <c r="H31" s="43">
+      <c r="H31" s="41">
         <f t="shared" si="5"/>
         <v>354.02769785043228</v>
       </c>
-      <c r="I31" s="44">
+      <c r="I31" s="42">
         <f t="shared" si="6"/>
         <v>174.87923902659878</v>
       </c>
@@ -2420,15 +2246,15 @@
         <f t="shared" si="3"/>
         <v>174.87923902659878</v>
       </c>
-      <c r="G32" s="42">
+      <c r="G32" s="40">
         <f t="shared" si="4"/>
         <v>2.8995856764676927E-3</v>
       </c>
-      <c r="H32" s="43">
+      <c r="H32" s="41">
         <f t="shared" si="5"/>
         <v>354.02776403462366</v>
       </c>
-      <c r="I32" s="44">
+      <c r="I32" s="42">
         <f t="shared" si="6"/>
         <v>174.87920688379387</v>
       </c>
@@ -2443,15 +2269,15 @@
         <f>I32</f>
         <v>174.87920688379387</v>
       </c>
-      <c r="G33" s="42">
+      <c r="G33" s="40">
         <f>0.0035*(F33-$C$25)/F33</f>
         <v>2.8995855661115171E-3</v>
       </c>
-      <c r="H33" s="43">
+      <c r="H33" s="41">
         <f>IF($B$3=415,-109.1569+537276.6*G33-250905000*G33^2+55282490000*G33^3-4709357000000*G33^4,1707.624-2356626*G33-1444077000*G33^2+366690400000*G33^3-33180890000000*G33^4)</f>
         <v>354.02776211607318</v>
       </c>
-      <c r="I33" s="44">
+      <c r="I33" s="42">
         <f>($A$32*$B$32-(H33-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
         <v>174.87920781555101</v>
       </c>
@@ -2466,15 +2292,15 @@
         <f>I33</f>
         <v>174.87920781555101</v>
       </c>
-      <c r="G34" s="42">
+      <c r="G34" s="40">
         <f>0.0035*(F34-$C$25)/F34</f>
         <v>2.8995855693105272E-3</v>
       </c>
-      <c r="H34" s="43">
+      <c r="H34" s="41">
         <f>IF($B$3=415,-109.1569+537276.6*G34-250905000*G34^2+55282490000*G34^3-4709357000000*G34^4,1707.624-2356626*G34-1444077000*G34^2+366690400000*G34^3-33180890000000*G34^4)</f>
         <v>354.02776217168855</v>
       </c>
-      <c r="I34" s="44">
+      <c r="I34" s="42">
         <f>($A$32*$B$32-(H34-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
         <v>174.87920778854104</v>
       </c>
@@ -2496,15 +2322,15 @@
         <f t="shared" ref="F35:F37" si="7">I34</f>
         <v>174.87920778854104</v>
       </c>
-      <c r="G35" s="42">
+      <c r="G35" s="40">
         <f t="shared" ref="G35:G37" si="8">0.0035*(F35-$C$25)/F35</f>
         <v>2.8995855692177941E-3</v>
       </c>
-      <c r="H35" s="43">
+      <c r="H35" s="41">
         <f t="shared" ref="H35:H37" si="9">IF($B$3=415,-109.1569+537276.6*G35-250905000*G35^2+55282490000*G35^3-4709357000000*G35^4,1707.624-2356626*G35-1444077000*G35^2+366690400000*G35^3-33180890000000*G35^4)</f>
         <v>354.02776217007596</v>
       </c>
-      <c r="I35" s="44">
+      <c r="I35" s="42">
         <f t="shared" ref="I35:I37" si="10">($A$32*$B$32-(H35-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
         <v>174.8792077893242</v>
       </c>
@@ -2519,15 +2345,15 @@
         <f t="shared" si="7"/>
         <v>174.8792077893242</v>
       </c>
-      <c r="G36" s="42">
+      <c r="G36" s="40">
         <f t="shared" si="8"/>
         <v>2.8995855692204829E-3</v>
       </c>
-      <c r="H36" s="43">
+      <c r="H36" s="41">
         <f t="shared" si="9"/>
         <v>354.02776217012297</v>
       </c>
-      <c r="I36" s="44">
+      <c r="I36" s="42">
         <f t="shared" si="10"/>
         <v>174.87920778930135</v>
       </c>
@@ -2542,15 +2368,15 @@
         <f t="shared" si="7"/>
         <v>174.87920778930135</v>
       </c>
-      <c r="G37" s="42">
+      <c r="G37" s="40">
         <f t="shared" si="8"/>
         <v>2.8995855692204048E-3</v>
       </c>
-      <c r="H37" s="43">
+      <c r="H37" s="41">
         <f t="shared" si="9"/>
         <v>354.02776217012172</v>
       </c>
-      <c r="I37" s="44">
+      <c r="I37" s="42">
         <f t="shared" si="10"/>
         <v>174.87920778930197</v>
       </c>
@@ -2561,67 +2387,368 @@
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
       <c r="E38" s="38"/>
-      <c r="F38" s="45">
+      <c r="F38" s="43">
         <f>I37</f>
         <v>174.87920778930197</v>
       </c>
-      <c r="G38" s="46">
+      <c r="G38" s="44">
         <f>0.0035*(F38-$C$25)/F38</f>
         <v>2.8995855692204066E-3</v>
       </c>
-      <c r="H38" s="47">
+      <c r="H38" s="45">
         <f>IF($B$3=415,-109.1569+537276.6*G38-250905000*G38^2+55282490000*G38^3-4709357000000*G38^4,1707.624-2356626*G38-1444077000*G38^2+366690400000*G38^3-33180890000000*G38^4)</f>
         <v>354.02776217012138</v>
       </c>
-      <c r="I38" s="48">
+      <c r="I38" s="46">
         <f>($A$32*$B$32-(H38-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
         <v>174.87920778930211</v>
       </c>
     </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="17"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="54" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42">
+        <v>200</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="str" cm="1">
+        <f t="array" ref="F42:G48">TRANSPOSE(A2:G3)</f>
+        <v>fck</v>
+      </c>
+      <c r="G42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>230</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" t="str">
+        <v>fy</v>
+      </c>
+      <c r="G43">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44">
+        <v>700</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="str">
+        <v>xu/d lim</v>
+      </c>
+      <c r="G44">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" t="str">
+        <v>j</v>
+      </c>
+      <c r="G45">
+        <v>0.8</v>
+      </c>
+    </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="7"/>
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" t="str">
+        <v>k1</v>
+      </c>
+      <c r="G46">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47">
+        <f>C44-C45-C46/2</f>
+        <v>640</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="str">
+        <v>k2 or Mu lim</v>
+      </c>
+      <c r="G47">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48">
+        <f>SQRT(C42*1000000/(G47*G42*C43))</f>
+        <v>561.30193423295896</v>
+      </c>
+      <c r="F48" t="str">
+        <v>pt lim*fy/fck</v>
+      </c>
+      <c r="G48">
+        <v>19.82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1000</v>
+      </c>
+      <c r="B52" s="48">
+        <f>0.87*$B$3*A52/(0.36*$A$3*$C$43)</f>
+        <v>218.02536231884062</v>
+      </c>
+      <c r="C52" s="48">
+        <f>$C$42*1000000/(0.87*$B$3*($C$47-0.416*B52))</f>
+        <v>1008.4442672632225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="48">
+        <f>C52</f>
+        <v>1008.4442672632225</v>
+      </c>
+      <c r="B53" s="48">
+        <f t="shared" ref="B53:B58" si="11">0.87*$B$3*A53/(0.36*$A$3*$C$43)</f>
+        <v>219.86642674842184</v>
+      </c>
+      <c r="C53" s="48">
+        <f t="shared" ref="C53:C58" si="12">$C$42*1000000/(0.87*$B$3*($C$47-0.416*B53))</f>
+        <v>1009.8522892202139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="48">
+        <f t="shared" ref="A54:A58" si="13">C53</f>
+        <v>1009.8522892202139</v>
+      </c>
+      <c r="B54" s="48">
+        <f t="shared" si="11"/>
+        <v>220.17341124574776</v>
+      </c>
+      <c r="C54" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.0874494943448</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.0874494943448</v>
+      </c>
+      <c r="B55" s="48">
+        <f t="shared" si="11"/>
+        <v>220.22468214971815</v>
+      </c>
+      <c r="C55" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1267353756164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.1267353756164</v>
+      </c>
+      <c r="B56" s="48">
+        <f t="shared" si="11"/>
+        <v>220.2332474682164</v>
+      </c>
+      <c r="C56" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1332987738311</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.1332987738311</v>
+      </c>
+      <c r="B57" s="48">
+        <f t="shared" si="11"/>
+        <v>220.23467845549021</v>
+      </c>
+      <c r="C57" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1343953133869</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.1343953133869</v>
+      </c>
+      <c r="B58" s="48">
+        <f t="shared" si="11"/>
+        <v>220.23491752892417</v>
+      </c>
+      <c r="C58" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1345785112489</v>
+      </c>
+      <c r="F58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G58" s="48">
+        <f>C58</f>
+        <v>1010.1345785112489</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="48">
+        <f>MAX(G41,G58)</f>
+        <v>1010.1345785112489</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="50">
+        <f>C46</f>
+        <v>20</v>
+      </c>
+      <c r="C61" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F61" s="55">
+        <f>ROUNDUP(C60/(B61^2*PI()/4),0)</f>
+        <v>4</v>
+      </c>
+      <c r="G61" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61" s="50">
+        <f>(C43-25*2)/(F61)</f>
+        <v>45</v>
+      </c>
+      <c r="I61" s="51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62">
+        <f>F61*PI()*B61^2/4</f>
+        <v>1256.6370614359173</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:N11">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="between">
       <formula>$D$11</formula>
       <formula>$B$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"over-reinforced"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>$C$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>$C$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>$B$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19 E15">
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="lessThan">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46 I28:I38">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="greaterThan">
+  <conditionalFormatting sqref="I28:I40">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="greaterThan">
       <formula>$C$29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:I38">
+  <conditionalFormatting sqref="I28:I40">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>$C$29</formula>
     </cfRule>
@@ -2634,4 +2761,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACD9705-F556-445F-B80D-CC394AB6BEE7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Beam design update and cantilever retaining wall design (#2)
* added doubly reinforced rcc beam design

* 1. added provision to calculate reinforcement in a singly reinforced beam
2. Cantilever retaining wall design. Procedure followed from Subramanyam RCC book
3. Corresponding autocad drawing of cantilever retaining wall
</commit_message>
<xml_diff>
--- a/Structural design sheets/Beam design.xlsx
+++ b/Structural design sheets/Beam design.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Structural design sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Exceldesignfiles\Structural design sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07D6F71-C171-4C74-A4B1-56D1B3A93768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F751061-6297-4136-8668-8DDDFA760EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{080EB4DA-FCC7-4271-9359-BF29FD8446FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Steel" sheetId="1" r:id="rId1"/>
     <sheet name="RCC" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="bf">Steel!$C$3</definedName>
@@ -46,7 +47,7 @@
     <author>Samyak</author>
   </authors>
   <commentList>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{A94A0C6E-5B0B-4D0F-B511-9E983DEA732B}">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{A94A0C6E-5B0B-4D0F-B511-9E983DEA732B}">
       <text>
         <r>
           <rPr>
@@ -74,8 +75,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>I - section</t>
   </si>
@@ -245,18 +268,6 @@
     <t>No of Rebar</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Rectangular beam, singly reinforced</t>
   </si>
   <si>
@@ -276,14 +287,100 @@
   </si>
   <si>
     <t>section moment calculation</t>
+  </si>
+  <si>
+    <t>Rectangular beam, doubly reinforced</t>
+  </si>
+  <si>
+    <t>d'</t>
+  </si>
+  <si>
+    <t>cover (t)</t>
+  </si>
+  <si>
+    <t>Compression reinforcement</t>
+  </si>
+  <si>
+    <t>Tension reinforcement</t>
+  </si>
+  <si>
+    <t>Asc provided</t>
+  </si>
+  <si>
+    <t>Esc</t>
+  </si>
+  <si>
+    <t>fsc</t>
+  </si>
+  <si>
+    <t>fcc</t>
+  </si>
+  <si>
+    <t>fst</t>
+  </si>
+  <si>
+    <t>xu lim</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>kNm</t>
+  </si>
+  <si>
+    <t>Ast</t>
+  </si>
+  <si>
+    <t>Ast'=Mu/0.87fy(d-0.416xu)</t>
+  </si>
+  <si>
+    <t>Ast for moment</t>
+  </si>
+  <si>
+    <t>Ast required=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provide </t>
+  </si>
+  <si>
+    <t>Ast provided =</t>
+  </si>
+  <si>
+    <t>Mu required</t>
+  </si>
+  <si>
+    <t>clear cover</t>
+  </si>
+  <si>
+    <t>use bar of dia</t>
+  </si>
+  <si>
+    <t>d min</t>
+  </si>
+  <si>
+    <t>Find Ast in singly reinforced beam for a given Mu and beam width</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>no of bars=</t>
+  </si>
+  <si>
+    <t>spacing=</t>
+  </si>
+  <si>
+    <t>mm c/c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -329,7 +426,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -353,9 +450,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -366,7 +461,44 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -374,7 +506,71 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -387,9 +583,46 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -398,42 +631,86 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -453,28 +730,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -512,76 +819,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -938,7 +1175,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,10 +1400,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF0584A-E401-4C04-B945-1304245BCBFF}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <pane ySplit="3" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,12 +1413,13 @@
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1209,7 +1448,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>415</v>
@@ -1235,19 +1474,24 @@
         <v>19.82</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>42</v>
       </c>
       <c r="R4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="19"/>
+      <c r="A5" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1256,29 +1500,17 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="18" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="27"/>
+      <c r="I6" s="15" t="s">
         <v>55</v>
       </c>
       <c r="J6" s="6">
@@ -1297,339 +1529,1228 @@
         <v>32</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>300</v>
-      </c>
-      <c r="B7" s="13">
-        <f>SQRT(E7*1000000/(F3*A3*A7))</f>
-        <v>491.47318718299044</v>
-      </c>
-      <c r="C7" s="6">
-        <v>650</v>
-      </c>
-      <c r="D7">
-        <f>C7+50</f>
-        <v>700</v>
-      </c>
-      <c r="E7">
+      <c r="A7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="15">
+        <v>2</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" ref="J7:N11" si="0">PI()*J$6^2/4*$I7</f>
+        <v>226.1946710584651</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="0"/>
+        <v>402.12385965949352</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="0"/>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="0"/>
+        <v>981.74770424681037</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="0"/>
+        <v>1608.4954386379741</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>230</v>
+      </c>
+      <c r="B8" s="11">
+        <f>SQRT(E8*1000000/(F3*A3*A8))</f>
+        <v>627.55464042350627</v>
+      </c>
+      <c r="C8" s="6">
+        <v>675</v>
+      </c>
+      <c r="D8" s="12">
+        <f>C8+50</f>
+        <v>725</v>
+      </c>
+      <c r="E8" s="12">
         <v>250</v>
       </c>
-      <c r="F7">
-        <f>F3*A3*A7*C7^2/1000000</f>
-        <v>437.28750000000002</v>
-      </c>
-      <c r="I7" s="18">
-        <v>2</v>
-      </c>
-      <c r="J7" s="17">
-        <f>PI()*J$6^2/4*$I7</f>
-        <v>226.1946710584651</v>
-      </c>
-      <c r="K7" s="17">
-        <f>PI()*K$6^2/4*$I7</f>
-        <v>402.12385965949352</v>
-      </c>
-      <c r="L7" s="17">
-        <f>PI()*L$6^2/4*$I7</f>
-        <v>628.31853071795865</v>
-      </c>
-      <c r="M7" s="17">
-        <f>PI()*M$6^2/4*$I7</f>
-        <v>981.74770424681037</v>
-      </c>
-      <c r="N7" s="17">
-        <f>PI()*N$6^2/4*$I7</f>
-        <v>1608.4954386379741</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>29</v>
+      <c r="F8" s="27">
+        <f>F3*A3*A8*C8^2/1000000</f>
+        <v>289.23075000000006</v>
       </c>
       <c r="I8" s="6">
         <v>3</v>
       </c>
-      <c r="J8" s="17">
-        <f>PI()*J$6^2/4*$I8</f>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
         <v>339.29200658769764</v>
       </c>
-      <c r="K8" s="17">
-        <f>PI()*K$6^2/4*$I8</f>
+      <c r="K8" s="14">
+        <f t="shared" si="0"/>
         <v>603.18578948924028</v>
       </c>
-      <c r="L8" s="17">
-        <f>PI()*L$6^2/4*$I8</f>
+      <c r="L8" s="14">
+        <f t="shared" si="0"/>
         <v>942.47779607693792</v>
       </c>
-      <c r="M8" s="17">
-        <f>PI()*M$6^2/4*$I8</f>
+      <c r="M8" s="14">
+        <f t="shared" si="0"/>
         <v>1472.6215563702156</v>
       </c>
-      <c r="N8" s="17">
-        <f>PI()*N$6^2/4*$I8</f>
+      <c r="N8" s="14">
+        <f t="shared" si="0"/>
         <v>2412.7431579569611</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="27"/>
       <c r="I9" s="6">
         <v>4</v>
       </c>
-      <c r="J9" s="17">
-        <f>PI()*J$6^2/4*$I9</f>
+      <c r="J9" s="14">
+        <f t="shared" si="0"/>
         <v>452.38934211693021</v>
       </c>
-      <c r="K9" s="17">
-        <f>PI()*K$6^2/4*$I9</f>
+      <c r="K9" s="14">
+        <f t="shared" si="0"/>
         <v>804.24771931898704</v>
       </c>
-      <c r="L9" s="17">
-        <f>PI()*L$6^2/4*$I9</f>
+      <c r="L9" s="14">
+        <f t="shared" si="0"/>
         <v>1256.6370614359173</v>
       </c>
-      <c r="M9" s="17">
-        <f>PI()*M$6^2/4*$I9</f>
+      <c r="M9" s="14">
+        <f t="shared" si="0"/>
         <v>1963.4954084936207</v>
       </c>
-      <c r="N9" s="17">
-        <f>PI()*N$6^2/4*$I9</f>
+      <c r="N9" s="14">
+        <f t="shared" si="0"/>
         <v>3216.9908772759482</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <f>G3*A3/B3</f>
-        <v>1.1939759036144579</v>
-      </c>
-      <c r="B10" s="7">
-        <f>A10/100*A7*C7</f>
-        <v>2328.2530120481929</v>
-      </c>
-      <c r="C10" s="17">
-        <v>1256.6400000000001</v>
-      </c>
-      <c r="D10" s="7">
-        <f>MAX(0.25*SQRT(A3)/B3,1.4/B3)*A7*C7</f>
-        <v>657.83132530120474</v>
-      </c>
-      <c r="E10" t="str">
-        <f>IF(C10&lt;B10, "under-reinforced","over-reinforced")</f>
-        <v>under-reinforced</v>
-      </c>
+      <c r="A10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="27"/>
       <c r="I10" s="6">
         <v>5</v>
       </c>
-      <c r="J10" s="17">
-        <f>PI()*J$6^2/4*$I10</f>
+      <c r="J10" s="14">
+        <f t="shared" si="0"/>
         <v>565.48667764616278</v>
       </c>
-      <c r="K10" s="17">
-        <f>PI()*K$6^2/4*$I10</f>
+      <c r="K10" s="14">
+        <f t="shared" si="0"/>
         <v>1005.3096491487338</v>
       </c>
-      <c r="L10" s="17">
-        <f>PI()*L$6^2/4*$I10</f>
+      <c r="L10" s="14">
+        <f t="shared" si="0"/>
         <v>1570.7963267948967</v>
       </c>
-      <c r="M10" s="17">
-        <f>PI()*M$6^2/4*$I10</f>
+      <c r="M10" s="14">
+        <f t="shared" si="0"/>
         <v>2454.3692606170262</v>
       </c>
-      <c r="N10" s="17">
-        <f>PI()*N$6^2/4*$I10</f>
+      <c r="N10" s="14">
+        <f t="shared" si="0"/>
         <v>4021.2385965949352</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="30">
+        <f>G3*A3/B3</f>
+        <v>0.95518072289156619</v>
+      </c>
+      <c r="B11" s="11">
+        <f>A11/100*A8*C8</f>
+        <v>1482.9180722891565</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1256.6400000000001</v>
+      </c>
+      <c r="D11" s="11">
+        <f>MAX(0.25*SQRT(A3)/B3,1.4/B3)*A8*C8</f>
+        <v>523.73493975903614</v>
+      </c>
+      <c r="E11" s="12" t="str">
+        <f>IF(C11&lt;B11, "under-reinforced","over-reinforced")</f>
+        <v>under-reinforced</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="I11" s="15">
+        <v>6</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="0"/>
+        <v>678.58401317539528</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="0"/>
+        <v>1206.3715789784806</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="0"/>
+        <v>1884.9555921538758</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="0"/>
+        <v>2945.2431127404311</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="0"/>
+        <v>4825.4863159139222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <f>0.87*B3*C11</f>
+        <v>453709.87200000003</v>
+      </c>
+      <c r="B15" s="13">
+        <f>0.36*A3*A8</f>
+        <v>1655.9999999999998</v>
+      </c>
+      <c r="C15" s="17">
+        <f>A15/B15</f>
+        <v>273.97939130434787</v>
+      </c>
+      <c r="D15" s="17">
+        <f>C8*(1-0.416*C15/C8)</f>
+        <v>561.02457321739132</v>
+      </c>
+      <c r="E15" s="20">
+        <f>A15*D15/1000000</f>
+        <v>254.54238730331724</v>
+      </c>
+      <c r="F15" s="36">
+        <f>C15/C8</f>
+        <v>0.40589539452495982</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="27"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="33"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="35">
+        <f>0.87*B3*C11</f>
+        <v>453709.87200000003</v>
+      </c>
+      <c r="B19" s="13">
+        <f>0.45*A3*A8</f>
+        <v>2070</v>
+      </c>
+      <c r="C19" s="17">
+        <f>A19/B19</f>
+        <v>219.18351304347829</v>
+      </c>
+      <c r="D19" s="17">
+        <f>C8-C19/2</f>
+        <v>565.40824347826083</v>
+      </c>
+      <c r="E19" s="21">
+        <f>A19*D19/1000000</f>
+        <v>256.53130177626656</v>
+      </c>
+      <c r="F19" s="36">
+        <f>C19/C8</f>
+        <v>0.32471631561996783</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="27"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
+        <v>230</v>
+      </c>
+      <c r="B25" s="6">
+        <v>500</v>
+      </c>
+      <c r="C25" s="12">
+        <v>30</v>
+      </c>
+      <c r="D25" s="12">
+        <v>50</v>
+      </c>
+      <c r="E25" s="12">
+        <f>B25+D25</f>
+        <v>550</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="27"/>
+      <c r="K25" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" s="6">
+        <v>12</v>
+      </c>
+      <c r="M25" s="6">
+        <v>16</v>
+      </c>
+      <c r="N25" s="6">
+        <v>20</v>
+      </c>
+      <c r="O25" s="6">
+        <v>25</v>
+      </c>
+      <c r="P25" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="27"/>
+      <c r="K26" s="15">
+        <v>2</v>
+      </c>
+      <c r="L26" s="14">
+        <f>PI()*L$25^2/4*$K26</f>
+        <v>226.1946710584651</v>
+      </c>
+      <c r="M26" s="14">
+        <f t="shared" ref="M26:P30" si="1">PI()*M$25^2/4*$K26</f>
+        <v>402.12385965949352</v>
+      </c>
+      <c r="N26" s="14">
+        <f t="shared" si="1"/>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="O26" s="14">
+        <f t="shared" si="1"/>
+        <v>981.74770424681037</v>
+      </c>
+      <c r="P26" s="14">
+        <f t="shared" si="1"/>
+        <v>1608.4954386379741</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="14"/>
-      <c r="I11" s="18">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="6">
+        <v>3</v>
+      </c>
+      <c r="L27" s="14">
+        <f t="shared" ref="L27:L30" si="2">PI()*L$25^2/4*$K27</f>
+        <v>339.29200658769764</v>
+      </c>
+      <c r="M27" s="14">
+        <f t="shared" si="1"/>
+        <v>603.18578948924028</v>
+      </c>
+      <c r="N27" s="14">
+        <f t="shared" si="1"/>
+        <v>942.47779607693792</v>
+      </c>
+      <c r="O27" s="14">
+        <f t="shared" si="1"/>
+        <v>1472.6215563702156</v>
+      </c>
+      <c r="P27" s="14">
+        <f t="shared" si="1"/>
+        <v>2412.7431579569611</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12">
+        <f>C29</f>
+        <v>239.5</v>
+      </c>
+      <c r="G28" s="40">
+        <f>0.0035*(F28-$C$25)/F28</f>
+        <v>3.0615866388308982E-3</v>
+      </c>
+      <c r="H28" s="41">
+        <f>IF($B$3=415,-109.1569+537276.6*G28-250905000*G28^2+55282490000*G28^3-4709357000000*G28^4,1707.624-2356626*G28-1444077000*G28^2+366690400000*G28^3-33180890000000*G28^4)</f>
+        <v>356.6447401411944</v>
+      </c>
+      <c r="I28" s="42">
+        <f>($A$32*$B$32-(H28-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>173.60825454972272</v>
+      </c>
+      <c r="K28" s="6">
+        <v>4</v>
+      </c>
+      <c r="L28" s="14">
+        <f t="shared" si="2"/>
+        <v>452.38934211693021</v>
+      </c>
+      <c r="M28" s="14">
+        <f t="shared" si="1"/>
+        <v>804.24771931898704</v>
+      </c>
+      <c r="N28" s="14">
+        <f t="shared" si="1"/>
+        <v>1256.6370614359173</v>
+      </c>
+      <c r="O28" s="14">
+        <f t="shared" si="1"/>
+        <v>1963.4954084936207</v>
+      </c>
+      <c r="P28" s="14">
+        <f t="shared" si="1"/>
+        <v>3216.9908772759482</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <f>M28</f>
+        <v>804.24771931898704</v>
+      </c>
+      <c r="B29" s="12">
+        <f>0.447*A3</f>
+        <v>8.94</v>
+      </c>
+      <c r="C29" s="12">
+        <f>C3*B25</f>
+        <v>239.5</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="11">
+        <f>I28</f>
+        <v>173.60825454972272</v>
+      </c>
+      <c r="G29" s="40">
+        <f>0.0035*(F29-$C$25)/F29</f>
+        <v>2.8951900485818939E-3</v>
+      </c>
+      <c r="H29" s="41">
+        <f>IF($B$3=415,-109.1569+537276.6*G29-250905000*G29^2+55282490000*G29^3-4709357000000*G29^4,1707.624-2356626*G29-1444077000*G29^2+366690400000*G29^3-33180890000000*G29^4)</f>
+        <v>353.95119915899562</v>
+      </c>
+      <c r="I29" s="42">
+        <f>($A$32*$B$32-(H29-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.91639113898938</v>
+      </c>
+      <c r="K29" s="6">
+        <v>5</v>
+      </c>
+      <c r="L29" s="14">
+        <f t="shared" si="2"/>
+        <v>565.48667764616278</v>
+      </c>
+      <c r="M29" s="14">
+        <f t="shared" si="1"/>
+        <v>1005.3096491487338</v>
+      </c>
+      <c r="N29" s="14">
+        <f t="shared" si="1"/>
+        <v>1570.7963267948967</v>
+      </c>
+      <c r="O29" s="14">
+        <f t="shared" si="1"/>
+        <v>2454.3692606170262</v>
+      </c>
+      <c r="P29" s="14">
+        <f t="shared" si="1"/>
+        <v>4021.2385965949352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="11">
+        <f t="shared" ref="F30:F32" si="3">I29</f>
+        <v>174.91639113898938</v>
+      </c>
+      <c r="G30" s="40">
+        <f t="shared" ref="G30:G32" si="4">0.0035*(F30-$C$25)/F30</f>
+        <v>2.8997132040269086E-3</v>
+      </c>
+      <c r="H30" s="41">
+        <f t="shared" ref="H30:H32" si="5">IF($B$3=415,-109.1569+537276.6*G30-250905000*G30^2+55282490000*G30^3-4709357000000*G30^4,1707.624-2356626*G30-1444077000*G30^2+366690400000*G30^3-33180890000000*G30^4)</f>
+        <v>354.02998098735662</v>
+      </c>
+      <c r="I30" s="42">
+        <f t="shared" ref="I30:I32" si="6">($A$32*$B$32-(H30-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87813020554546</v>
+      </c>
+      <c r="K30" s="15">
         <v>6</v>
       </c>
-      <c r="J11" s="17">
-        <f>PI()*J$6^2/4*$I11</f>
+      <c r="L30" s="14">
+        <f t="shared" si="2"/>
         <v>678.58401317539528</v>
       </c>
-      <c r="K11" s="17">
-        <f>PI()*K$6^2/4*$I11</f>
+      <c r="M30" s="14">
+        <f t="shared" si="1"/>
         <v>1206.3715789784806</v>
       </c>
-      <c r="L11" s="17">
-        <f>PI()*L$6^2/4*$I11</f>
+      <c r="N30" s="14">
+        <f t="shared" si="1"/>
         <v>1884.9555921538758</v>
       </c>
-      <c r="M11" s="17">
-        <f>PI()*M$6^2/4*$I11</f>
+      <c r="O30" s="14">
+        <f t="shared" si="1"/>
         <v>2945.2431127404311</v>
       </c>
-      <c r="N11" s="17">
-        <f>PI()*N$6^2/4*$I11</f>
+      <c r="P30" s="14">
+        <f t="shared" si="1"/>
         <v>4825.4863159139222</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="11" t="s">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="11">
+        <f t="shared" si="3"/>
+        <v>174.87813020554546</v>
+      </c>
+      <c r="G31" s="40">
+        <f t="shared" si="4"/>
+        <v>2.8995818695191516E-3</v>
+      </c>
+      <c r="H31" s="41">
+        <f t="shared" si="5"/>
+        <v>354.02769785043228</v>
+      </c>
+      <c r="I31" s="42">
+        <f t="shared" si="6"/>
+        <v>174.87923902659878</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <f>N29</f>
+        <v>1570.7963267948967</v>
+      </c>
+      <c r="B32" s="12">
+        <f>0.87*B3</f>
+        <v>361.05</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="11">
+        <f t="shared" si="3"/>
+        <v>174.87923902659878</v>
+      </c>
+      <c r="G32" s="40">
+        <f t="shared" si="4"/>
+        <v>2.8995856764676927E-3</v>
+      </c>
+      <c r="H32" s="41">
+        <f t="shared" si="5"/>
+        <v>354.02776403462366</v>
+      </c>
+      <c r="I32" s="42">
+        <f t="shared" si="6"/>
+        <v>174.87920688379387</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="11">
+        <f>I32</f>
+        <v>174.87920688379387</v>
+      </c>
+      <c r="G33" s="40">
+        <f>0.0035*(F33-$C$25)/F33</f>
+        <v>2.8995855661115171E-3</v>
+      </c>
+      <c r="H33" s="41">
+        <f>IF($B$3=415,-109.1569+537276.6*G33-250905000*G33^2+55282490000*G33^3-4709357000000*G33^4,1707.624-2356626*G33-1444077000*G33^2+366690400000*G33^3-33180890000000*G33^4)</f>
+        <v>354.02776211607318</v>
+      </c>
+      <c r="I33" s="42">
+        <f>($A$32*$B$32-(H33-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87920781555101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="11">
+        <f>I33</f>
+        <v>174.87920781555101</v>
+      </c>
+      <c r="G34" s="40">
+        <f>0.0035*(F34-$C$25)/F34</f>
+        <v>2.8995855693105272E-3</v>
+      </c>
+      <c r="H34" s="41">
+        <f>IF($B$3=415,-109.1569+537276.6*G34-250905000*G34^2+55282490000*G34^3-4709357000000*G34^4,1707.624-2356626*G34-1444077000*G34^2+366690400000*G34^3-33180890000000*G34^4)</f>
+        <v>354.02776217168855</v>
+      </c>
+      <c r="I34" s="42">
+        <f>($A$32*$B$32-(H34-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87920778854104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="11">
+        <f>(0.36*A3*A25*I38*(B25-0.416*I38)+(H38-B29)*A29*(B25-C25))/1000000</f>
+        <v>254.17360011720072</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="11">
+        <f t="shared" ref="F35:F37" si="7">I34</f>
+        <v>174.87920778854104</v>
+      </c>
+      <c r="G35" s="40">
+        <f t="shared" ref="G35:G37" si="8">0.0035*(F35-$C$25)/F35</f>
+        <v>2.8995855692177941E-3</v>
+      </c>
+      <c r="H35" s="41">
+        <f t="shared" ref="H35:H37" si="9">IF($B$3=415,-109.1569+537276.6*G35-250905000*G35^2+55282490000*G35^3-4709357000000*G35^4,1707.624-2356626*G35-1444077000*G35^2+366690400000*G35^3-33180890000000*G35^4)</f>
+        <v>354.02776217007596</v>
+      </c>
+      <c r="I35" s="42">
+        <f t="shared" ref="I35:I37" si="10">($A$32*$B$32-(H35-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.8792077893242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="11">
+        <f t="shared" si="7"/>
+        <v>174.8792077893242</v>
+      </c>
+      <c r="G36" s="40">
+        <f t="shared" si="8"/>
+        <v>2.8995855692204829E-3</v>
+      </c>
+      <c r="H36" s="41">
+        <f t="shared" si="9"/>
+        <v>354.02776217012297</v>
+      </c>
+      <c r="I36" s="42">
+        <f t="shared" si="10"/>
+        <v>174.87920778930135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="11">
+        <f t="shared" si="7"/>
+        <v>174.87920778930135</v>
+      </c>
+      <c r="G37" s="40">
+        <f t="shared" si="8"/>
+        <v>2.8995855692204048E-3</v>
+      </c>
+      <c r="H37" s="41">
+        <f t="shared" si="9"/>
+        <v>354.02776217012172</v>
+      </c>
+      <c r="I37" s="42">
+        <f t="shared" si="10"/>
+        <v>174.87920778930197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="43">
+        <f>I37</f>
+        <v>174.87920778930197</v>
+      </c>
+      <c r="G38" s="44">
+        <f>0.0035*(F38-$C$25)/F38</f>
+        <v>2.8995855692204066E-3</v>
+      </c>
+      <c r="H38" s="45">
+        <f>IF($B$3=415,-109.1569+537276.6*G38-250905000*G38^2+55282490000*G38^3-4709357000000*G38^4,1707.624-2356626*G38-1444077000*G38^2+366690400000*G38^3-33180890000000*G38^4)</f>
+        <v>354.02776217012138</v>
+      </c>
+      <c r="I38" s="46">
+        <f>($A$32*$B$32-(H38-$B$29)*$A$29)/(0.36*$A$3*$A$25)</f>
+        <v>174.87920778930211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="17"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="54" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42">
+        <v>200</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="str" cm="1">
+        <f t="array" ref="F42:G48">TRANSPOSE(A2:G3)</f>
+        <v>fck</v>
+      </c>
+      <c r="G42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>230</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" t="str">
+        <v>fy</v>
+      </c>
+      <c r="G43">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44">
+        <v>700</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="str">
+        <v>xu/d lim</v>
+      </c>
+      <c r="G44">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" t="str">
+        <v>j</v>
+      </c>
+      <c r="G45">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" t="str">
+        <v>k1</v>
+      </c>
+      <c r="G46">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47">
+        <f>C44-C45-C46/2</f>
+        <v>640</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="str">
+        <v>k2 or Mu lim</v>
+      </c>
+      <c r="G47">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48">
+        <f>SQRT(C42*1000000/(G47*G42*C43))</f>
+        <v>561.30193423295896</v>
+      </c>
+      <c r="F48" t="str">
+        <v>pt lim*fy/fck</v>
+      </c>
+      <c r="G48">
+        <v>19.82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1000</v>
+      </c>
+      <c r="B52" s="48">
+        <f>0.87*$B$3*A52/(0.36*$A$3*$C$43)</f>
+        <v>218.02536231884062</v>
+      </c>
+      <c r="C52" s="48">
+        <f>$C$42*1000000/(0.87*$B$3*($C$47-0.416*B52))</f>
+        <v>1008.4442672632225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="48">
+        <f>C52</f>
+        <v>1008.4442672632225</v>
+      </c>
+      <c r="B53" s="48">
+        <f t="shared" ref="B53:B58" si="11">0.87*$B$3*A53/(0.36*$A$3*$C$43)</f>
+        <v>219.86642674842184</v>
+      </c>
+      <c r="C53" s="48">
+        <f t="shared" ref="C53:C58" si="12">$C$42*1000000/(0.87*$B$3*($C$47-0.416*B53))</f>
+        <v>1009.8522892202139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="48">
+        <f t="shared" ref="A54:A58" si="13">C53</f>
+        <v>1009.8522892202139</v>
+      </c>
+      <c r="B54" s="48">
+        <f t="shared" si="11"/>
+        <v>220.17341124574776</v>
+      </c>
+      <c r="C54" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.0874494943448</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.0874494943448</v>
+      </c>
+      <c r="B55" s="48">
+        <f t="shared" si="11"/>
+        <v>220.22468214971815</v>
+      </c>
+      <c r="C55" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1267353756164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.1267353756164</v>
+      </c>
+      <c r="B56" s="48">
+        <f t="shared" si="11"/>
+        <v>220.2332474682164</v>
+      </c>
+      <c r="C56" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1332987738311</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.1332987738311</v>
+      </c>
+      <c r="B57" s="48">
+        <f t="shared" si="11"/>
+        <v>220.23467845549021</v>
+      </c>
+      <c r="C57" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1343953133869</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="48">
+        <f t="shared" si="13"/>
+        <v>1010.1343953133869</v>
+      </c>
+      <c r="B58" s="48">
+        <f t="shared" si="11"/>
+        <v>220.23491752892417</v>
+      </c>
+      <c r="C58" s="48">
+        <f t="shared" si="12"/>
+        <v>1010.1345785112489</v>
+      </c>
+      <c r="F58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G58" s="48">
+        <f>C58</f>
+        <v>1010.1345785112489</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="48">
+        <f>MAX(G41,G58)</f>
+        <v>1010.1345785112489</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="50">
+        <f>C46</f>
+        <v>20</v>
+      </c>
+      <c r="C61" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F61" s="55">
+        <f>ROUNDUP(C60/(B61^2*PI()/4),0)</f>
+        <v>4</v>
+      </c>
+      <c r="G61" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61" s="50">
+        <f>(C43-25*2)/(F61)</f>
         <v>45</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <f>0.87*B3*C10</f>
-        <v>453709.87200000003</v>
-      </c>
-      <c r="B14" s="16">
-        <f>0.36*A3*A7</f>
-        <v>2700</v>
-      </c>
-      <c r="C14" s="20">
-        <f>A14/B14</f>
-        <v>168.04069333333334</v>
-      </c>
-      <c r="D14" s="20">
-        <f>C7*(1-0.416*C14/C7)</f>
-        <v>580.09507157333337</v>
-      </c>
-      <c r="E14" s="24">
-        <f>A14*D14/1000000</f>
-        <v>263.19486067136796</v>
-      </c>
-      <c r="F14" s="22">
-        <f>C14/C7</f>
-        <v>0.25852414358974357</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <f>0.87*B3*C10</f>
-        <v>453709.87200000003</v>
-      </c>
-      <c r="B18" s="16">
-        <f>0.45*A3*A7</f>
-        <v>3375</v>
-      </c>
-      <c r="C18" s="20">
-        <f>A18/B18</f>
-        <v>134.43255466666668</v>
-      </c>
-      <c r="D18" s="20">
-        <f>C7-C18/2</f>
-        <v>582.78372266666668</v>
-      </c>
-      <c r="E18" s="25">
-        <f>A18*D18/1000000</f>
-        <v>264.41472821477686</v>
-      </c>
-      <c r="F18" s="22">
-        <f>C18/C7</f>
-        <v>0.20681931487179489</v>
+      <c r="I61" s="51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62">
+        <f>F61*PI()*B61^2/4</f>
+        <v>1256.6370614359173</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:N11">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
-      <formula>$D$10</formula>
-      <formula>$B$10</formula>
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="between">
+      <formula>$D$11</formula>
+      <formula>$B$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"over-reinforced"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
-      <formula>$C$10</formula>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+      <formula>$C$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
-      <formula>$C$10</formula>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
+      <formula>$C$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>$B$7</formula>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+      <formula>$B$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18 E14">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="lessThan">
-      <formula>$E$7</formula>
+  <conditionalFormatting sqref="E19 E15">
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="lessThan">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:I40">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="greaterThan">
+      <formula>$C$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:I40">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$C$29</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1640,4 +2761,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACD9705-F556-445F-B80D-CC394AB6BEE7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
delete company file, other minor changes
</commit_message>
<xml_diff>
--- a/Structural design sheets/Beam design.xlsx
+++ b/Structural design sheets/Beam design.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Exceldesignfiles\Structural design sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F751061-6297-4136-8668-8DDDFA760EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACB80B8-EEC2-469C-8CCA-461053521D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{080EB4DA-FCC7-4271-9359-BF29FD8446FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Steel" sheetId="1" r:id="rId1"/>
     <sheet name="RCC" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="bf">Steel!$C$3</definedName>
@@ -1404,7 +1403,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O63" sqref="O63"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2761,16 +2760,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACD9705-F556-445F-B80D-CC394AB6BEE7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>